<commit_message>
api com estado e municipio inclusos
</commit_message>
<xml_diff>
--- a/Bot-Varredura/dominios.xlsx
+++ b/Bot-Varredura/dominios.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C92"/>
+  <dimension ref="A1:E94"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,6 +449,16 @@
           <t>DATA EXTRACAO</t>
         </is>
       </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>MUNICIPIO</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>ESTADO</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -463,7 +473,17 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2025-01-15 13:42:57</t>
+          <t>2025-01-21 17:03:53</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Nova Friburgo</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro</t>
         </is>
       </c>
     </row>
@@ -480,7 +500,17 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2025-01-15 13:43:56</t>
+          <t>2025-01-21 12:57:19</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Bom Jardim</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro</t>
         </is>
       </c>
     </row>
@@ -500,6 +530,8 @@
           <t>2025-01-15 13:44:02</t>
         </is>
       </c>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -517,6 +549,8 @@
           <t>2025-01-15 13:44:09</t>
         </is>
       </c>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -534,6 +568,8 @@
           <t>2025-01-15 13:44:16</t>
         </is>
       </c>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -551,6 +587,8 @@
           <t>2025-01-15 13:45:18</t>
         </is>
       </c>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -568,6 +606,8 @@
           <t>2025-01-15 13:45:21</t>
         </is>
       </c>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -585,6 +625,8 @@
           <t>2025-01-15 13:45:33</t>
         </is>
       </c>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -602,6 +644,8 @@
           <t>2025-01-15 13:45:41</t>
         </is>
       </c>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -619,6 +663,8 @@
           <t>2025-01-15 13:47:02</t>
         </is>
       </c>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -636,6 +682,8 @@
           <t>2025-01-15 13:47:08</t>
         </is>
       </c>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -653,6 +701,8 @@
           <t>2025-01-15 13:47:20</t>
         </is>
       </c>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -670,6 +720,8 @@
           <t>2025-01-15 13:47:26</t>
         </is>
       </c>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -687,6 +739,8 @@
           <t>2025-01-15 13:47:35</t>
         </is>
       </c>
+      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -704,6 +758,8 @@
           <t>2025-01-15 13:47:36</t>
         </is>
       </c>
+      <c r="D16" t="inlineStr"/>
+      <c r="E16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -721,6 +777,8 @@
           <t>2025-01-15 13:47:42</t>
         </is>
       </c>
+      <c r="D17" t="inlineStr"/>
+      <c r="E17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -738,6 +796,8 @@
           <t>2025-01-15 13:47:53</t>
         </is>
       </c>
+      <c r="D18" t="inlineStr"/>
+      <c r="E18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -755,6 +815,8 @@
           <t>2025-01-15 13:47:57</t>
         </is>
       </c>
+      <c r="D19" t="inlineStr"/>
+      <c r="E19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -772,6 +834,8 @@
           <t>2025-01-15 13:48:02</t>
         </is>
       </c>
+      <c r="D20" t="inlineStr"/>
+      <c r="E20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -789,6 +853,8 @@
           <t>2025-01-15 13:48:16</t>
         </is>
       </c>
+      <c r="D21" t="inlineStr"/>
+      <c r="E21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -806,6 +872,8 @@
           <t>2025-01-15 13:48:22</t>
         </is>
       </c>
+      <c r="D22" t="inlineStr"/>
+      <c r="E22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -823,6 +891,8 @@
           <t>2025-01-15 13:48:41</t>
         </is>
       </c>
+      <c r="D23" t="inlineStr"/>
+      <c r="E23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -840,6 +910,8 @@
           <t>2025-01-15 13:48:51</t>
         </is>
       </c>
+      <c r="D24" t="inlineStr"/>
+      <c r="E24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -857,6 +929,8 @@
           <t>2025-01-15 13:49:23</t>
         </is>
       </c>
+      <c r="D25" t="inlineStr"/>
+      <c r="E25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -874,6 +948,8 @@
           <t>2025-01-15 13:49:31</t>
         </is>
       </c>
+      <c r="D26" t="inlineStr"/>
+      <c r="E26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -891,6 +967,8 @@
           <t>2025-01-15 13:49:36</t>
         </is>
       </c>
+      <c r="D27" t="inlineStr"/>
+      <c r="E27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -908,6 +986,8 @@
           <t>2025-01-15 13:50:23</t>
         </is>
       </c>
+      <c r="D28" t="inlineStr"/>
+      <c r="E28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -925,6 +1005,8 @@
           <t>2025-01-15 13:50:28</t>
         </is>
       </c>
+      <c r="D29" t="inlineStr"/>
+      <c r="E29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -942,6 +1024,8 @@
           <t>2025-01-15 13:50:38</t>
         </is>
       </c>
+      <c r="D30" t="inlineStr"/>
+      <c r="E30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -959,6 +1043,8 @@
           <t>2025-01-15 13:50:54</t>
         </is>
       </c>
+      <c r="D31" t="inlineStr"/>
+      <c r="E31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -976,6 +1062,8 @@
           <t>2025-01-15 13:51:06</t>
         </is>
       </c>
+      <c r="D32" t="inlineStr"/>
+      <c r="E32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -993,6 +1081,8 @@
           <t>2025-01-15 13:51:14</t>
         </is>
       </c>
+      <c r="D33" t="inlineStr"/>
+      <c r="E33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1010,6 +1100,8 @@
           <t>2025-01-15 13:51:14</t>
         </is>
       </c>
+      <c r="D34" t="inlineStr"/>
+      <c r="E34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1027,6 +1119,8 @@
           <t>2025-01-15 13:51:25</t>
         </is>
       </c>
+      <c r="D35" t="inlineStr"/>
+      <c r="E35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1044,6 +1138,8 @@
           <t>2025-01-15 13:51:25</t>
         </is>
       </c>
+      <c r="D36" t="inlineStr"/>
+      <c r="E36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1061,6 +1157,8 @@
           <t>2025-01-15 13:51:33</t>
         </is>
       </c>
+      <c r="D37" t="inlineStr"/>
+      <c r="E37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1078,6 +1176,8 @@
           <t>2025-01-15 13:51:33</t>
         </is>
       </c>
+      <c r="D38" t="inlineStr"/>
+      <c r="E38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1095,6 +1195,8 @@
           <t>2025-01-15 13:51:38</t>
         </is>
       </c>
+      <c r="D39" t="inlineStr"/>
+      <c r="E39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1112,6 +1214,8 @@
           <t>2025-01-15 13:51:44</t>
         </is>
       </c>
+      <c r="D40" t="inlineStr"/>
+      <c r="E40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -1129,6 +1233,8 @@
           <t>2025-01-15 13:51:53</t>
         </is>
       </c>
+      <c r="D41" t="inlineStr"/>
+      <c r="E41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -1146,6 +1252,8 @@
           <t>2025-01-15 13:52:01</t>
         </is>
       </c>
+      <c r="D42" t="inlineStr"/>
+      <c r="E42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -1163,6 +1271,8 @@
           <t>2025-01-15 13:52:12</t>
         </is>
       </c>
+      <c r="D43" t="inlineStr"/>
+      <c r="E43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -1180,6 +1290,8 @@
           <t>2025-01-15 13:52:25</t>
         </is>
       </c>
+      <c r="D44" t="inlineStr"/>
+      <c r="E44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -1197,6 +1309,8 @@
           <t>2025-01-15 13:52:37</t>
         </is>
       </c>
+      <c r="D45" t="inlineStr"/>
+      <c r="E45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -1214,6 +1328,8 @@
           <t>2025-01-15 13:52:46</t>
         </is>
       </c>
+      <c r="D46" t="inlineStr"/>
+      <c r="E46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -1231,6 +1347,8 @@
           <t>2025-01-15 13:53:16</t>
         </is>
       </c>
+      <c r="D47" t="inlineStr"/>
+      <c r="E47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -1248,6 +1366,8 @@
           <t>2025-01-15 13:53:24</t>
         </is>
       </c>
+      <c r="D48" t="inlineStr"/>
+      <c r="E48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -1265,6 +1385,8 @@
           <t>2025-01-15 13:53:31</t>
         </is>
       </c>
+      <c r="D49" t="inlineStr"/>
+      <c r="E49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -1282,6 +1404,8 @@
           <t>2025-01-15 13:53:32</t>
         </is>
       </c>
+      <c r="D50" t="inlineStr"/>
+      <c r="E50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -1299,6 +1423,8 @@
           <t>2025-01-15 13:53:38</t>
         </is>
       </c>
+      <c r="D51" t="inlineStr"/>
+      <c r="E51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -1316,6 +1442,8 @@
           <t>2025-01-15 13:53:45</t>
         </is>
       </c>
+      <c r="D52" t="inlineStr"/>
+      <c r="E52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -1333,6 +1461,8 @@
           <t>2025-01-15 13:53:51</t>
         </is>
       </c>
+      <c r="D53" t="inlineStr"/>
+      <c r="E53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -1350,6 +1480,8 @@
           <t>2025-01-15 13:54:00</t>
         </is>
       </c>
+      <c r="D54" t="inlineStr"/>
+      <c r="E54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -1367,6 +1499,8 @@
           <t>2025-01-15 13:54:06</t>
         </is>
       </c>
+      <c r="D55" t="inlineStr"/>
+      <c r="E55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -1384,6 +1518,8 @@
           <t>2025-01-15 13:54:15</t>
         </is>
       </c>
+      <c r="D56" t="inlineStr"/>
+      <c r="E56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -1401,6 +1537,8 @@
           <t>2025-01-15 13:54:25</t>
         </is>
       </c>
+      <c r="D57" t="inlineStr"/>
+      <c r="E57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -1418,6 +1556,8 @@
           <t>2025-01-15 13:54:41</t>
         </is>
       </c>
+      <c r="D58" t="inlineStr"/>
+      <c r="E58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -1435,6 +1575,8 @@
           <t>2025-01-15 13:54:47</t>
         </is>
       </c>
+      <c r="D59" t="inlineStr"/>
+      <c r="E59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -1452,6 +1594,8 @@
           <t>2025-01-15 13:54:53</t>
         </is>
       </c>
+      <c r="D60" t="inlineStr"/>
+      <c r="E60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -1469,6 +1613,8 @@
           <t>2025-01-15 13:54:58</t>
         </is>
       </c>
+      <c r="D61" t="inlineStr"/>
+      <c r="E61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -1486,6 +1632,8 @@
           <t>2025-01-15 13:55:30</t>
         </is>
       </c>
+      <c r="D62" t="inlineStr"/>
+      <c r="E62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -1503,6 +1651,8 @@
           <t>2025-01-15 13:55:35</t>
         </is>
       </c>
+      <c r="D63" t="inlineStr"/>
+      <c r="E63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -1520,6 +1670,8 @@
           <t>2025-01-15 13:55:41</t>
         </is>
       </c>
+      <c r="D64" t="inlineStr"/>
+      <c r="E64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -1537,6 +1689,8 @@
           <t>2025-01-15 13:55:50</t>
         </is>
       </c>
+      <c r="D65" t="inlineStr"/>
+      <c r="E65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -1554,6 +1708,8 @@
           <t>2025-01-15 13:55:57</t>
         </is>
       </c>
+      <c r="D66" t="inlineStr"/>
+      <c r="E66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -1571,6 +1727,8 @@
           <t>2025-01-15 13:56:04</t>
         </is>
       </c>
+      <c r="D67" t="inlineStr"/>
+      <c r="E67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -1588,6 +1746,8 @@
           <t>2025-01-15 13:56:09</t>
         </is>
       </c>
+      <c r="D68" t="inlineStr"/>
+      <c r="E68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -1605,6 +1765,8 @@
           <t>2025-01-15 13:56:30</t>
         </is>
       </c>
+      <c r="D69" t="inlineStr"/>
+      <c r="E69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -1622,6 +1784,8 @@
           <t>2025-01-15 13:56:36</t>
         </is>
       </c>
+      <c r="D70" t="inlineStr"/>
+      <c r="E70" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -1639,6 +1803,8 @@
           <t>2025-01-15 13:56:36</t>
         </is>
       </c>
+      <c r="D71" t="inlineStr"/>
+      <c r="E71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -1656,6 +1822,8 @@
           <t>2025-01-15 13:56:37</t>
         </is>
       </c>
+      <c r="D72" t="inlineStr"/>
+      <c r="E72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -1673,6 +1841,8 @@
           <t>2025-01-15 13:56:51</t>
         </is>
       </c>
+      <c r="D73" t="inlineStr"/>
+      <c r="E73" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -1690,6 +1860,8 @@
           <t>2025-01-15 13:57:03</t>
         </is>
       </c>
+      <c r="D74" t="inlineStr"/>
+      <c r="E74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -1707,6 +1879,8 @@
           <t>2025-01-15 13:57:03</t>
         </is>
       </c>
+      <c r="D75" t="inlineStr"/>
+      <c r="E75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -1724,6 +1898,8 @@
           <t>2025-01-15 13:57:17</t>
         </is>
       </c>
+      <c r="D76" t="inlineStr"/>
+      <c r="E76" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -1741,6 +1917,8 @@
           <t>2025-01-15 13:57:47</t>
         </is>
       </c>
+      <c r="D77" t="inlineStr"/>
+      <c r="E77" t="inlineStr"/>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -1758,6 +1936,8 @@
           <t>2025-01-15 13:58:01</t>
         </is>
       </c>
+      <c r="D78" t="inlineStr"/>
+      <c r="E78" t="inlineStr"/>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -1775,6 +1955,8 @@
           <t>2025-01-15 13:58:15</t>
         </is>
       </c>
+      <c r="D79" t="inlineStr"/>
+      <c r="E79" t="inlineStr"/>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -1792,6 +1974,8 @@
           <t>2025-01-15 14:00:12</t>
         </is>
       </c>
+      <c r="D80" t="inlineStr"/>
+      <c r="E80" t="inlineStr"/>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -1809,6 +1993,8 @@
           <t>2025-01-15 14:00:28</t>
         </is>
       </c>
+      <c r="D81" t="inlineStr"/>
+      <c r="E81" t="inlineStr"/>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -1826,6 +2012,8 @@
           <t>2025-01-15 14:00:37</t>
         </is>
       </c>
+      <c r="D82" t="inlineStr"/>
+      <c r="E82" t="inlineStr"/>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -1843,6 +2031,8 @@
           <t>2025-01-15 14:00:45</t>
         </is>
       </c>
+      <c r="D83" t="inlineStr"/>
+      <c r="E83" t="inlineStr"/>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -1860,6 +2050,8 @@
           <t>2025-01-15 14:01:01</t>
         </is>
       </c>
+      <c r="D84" t="inlineStr"/>
+      <c r="E84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -1877,6 +2069,8 @@
           <t>2025-01-15 14:01:13</t>
         </is>
       </c>
+      <c r="D85" t="inlineStr"/>
+      <c r="E85" t="inlineStr"/>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -1894,6 +2088,8 @@
           <t>2025-01-15 14:01:28</t>
         </is>
       </c>
+      <c r="D86" t="inlineStr"/>
+      <c r="E86" t="inlineStr"/>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -1911,6 +2107,8 @@
           <t>2025-01-15 14:01:37</t>
         </is>
       </c>
+      <c r="D87" t="inlineStr"/>
+      <c r="E87" t="inlineStr"/>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -1928,6 +2126,8 @@
           <t>2025-01-15 14:01:37</t>
         </is>
       </c>
+      <c r="D88" t="inlineStr"/>
+      <c r="E88" t="inlineStr"/>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -1945,6 +2145,8 @@
           <t>2025-01-15 14:01:37</t>
         </is>
       </c>
+      <c r="D89" t="inlineStr"/>
+      <c r="E89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -1962,6 +2164,8 @@
           <t>2025-01-15 14:01:45</t>
         </is>
       </c>
+      <c r="D90" t="inlineStr"/>
+      <c r="E90" t="inlineStr"/>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -1979,6 +2183,8 @@
           <t>2025-01-15 14:01:53</t>
         </is>
       </c>
+      <c r="D91" t="inlineStr"/>
+      <c r="E91" t="inlineStr"/>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -1994,6 +2200,62 @@
       <c r="C92" t="inlineStr">
         <is>
           <t>2025-01-15 14:02:22</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr"/>
+      <c r="E92" t="inlineStr"/>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>acrelandia.ac.gov.br</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>SUCESSO</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>2025-01-21 17:04:11</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>Acrelândia</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>Acre</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>assisbrasil.ac.gov.br</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>SUCESSO</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>2025-01-21 12:57:32</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>Assis Brasil</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>Acre</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
dropdown de estado adicionado
</commit_message>
<xml_diff>
--- a/Bot-Varredura/dominios.xlsx
+++ b/Bot-Varredura/dominios.xlsx
@@ -473,7 +473,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2025-01-21 17:03:53</t>
+          <t>2025-01-23 16:22:41</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -500,7 +500,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2025-01-21 12:57:19</t>
+          <t>2025-01-23 16:22:55</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -527,11 +527,19 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2025-01-15 13:44:02</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
+          <t>2025-01-23 16:23:01</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Cordeiro</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -2218,7 +2226,7 @@
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>2025-01-21 17:04:11</t>
+          <t>2025-01-23 16:23:08</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
@@ -2240,12 +2248,12 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>SUCESSO</t>
+          <t>ERRO</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>2025-01-21 12:57:32</t>
+          <t>2025-01-23 16:23:14</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">

</xml_diff>

<commit_message>
wcag e metodologia adicionados ao menu
</commit_message>
<xml_diff>
--- a/Bot-Varredura/dominios.xlsx
+++ b/Bot-Varredura/dominios.xlsx
@@ -473,7 +473,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2025-01-23 16:22:41</t>
+          <t>2025-01-25 19:07:18</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -500,7 +500,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2025-01-23 16:22:55</t>
+          <t>2025-01-25 17:10:47</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -527,7 +527,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2025-01-23 16:23:01</t>
+          <t>2025-01-25 16:31:01</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -630,7 +630,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>2025-01-15 13:45:33</t>
+          <t>2025-01-25 16:19:09</t>
         </is>
       </c>
       <c r="D9" t="inlineStr"/>
@@ -934,11 +934,19 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>2025-01-15 13:49:23</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr"/>
-      <c r="E25" t="inlineStr"/>
+          <t>2025-01-25 17:25:41</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Macaé</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1067,11 +1075,19 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>2025-01-15 13:51:06</t>
-        </is>
-      </c>
-      <c r="D32" t="inlineStr"/>
-      <c r="E32" t="inlineStr"/>
+          <t>2025-01-25 17:25:51</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Nova Iguaçu</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -1466,11 +1482,19 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>2025-01-15 13:53:51</t>
-        </is>
-      </c>
-      <c r="D53" t="inlineStr"/>
-      <c r="E53" t="inlineStr"/>
+          <t>2025-01-25 19:07:59</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>Teresópolis</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -2226,7 +2250,7 @@
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>2025-01-23 16:23:08</t>
+          <t>2025-01-25 17:10:54</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">

</xml_diff>

<commit_message>
bot varreduro com split e grafico com top 10
</commit_message>
<xml_diff>
--- a/Bot-Varredura/dominios.xlsx
+++ b/Bot-Varredura/dominios.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E95"/>
+  <dimension ref="A1:E93"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,7 +463,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>novafriburgo.rj.gov.br</t>
+          <t xml:space="preserve">angra.rj.gov.br </t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -473,12 +473,12 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2025-01-23 16:22:41</t>
+          <t>2025-01-31 10:24:15</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Nova Friburgo</t>
+          <t>Angra dos Reis</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -490,7 +490,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>bomjardim.rj.gov.br</t>
+          <t>aperibe.rj.gov.br</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -500,12 +500,12 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2025-01-29 12:28:29</t>
+          <t>2025-01-31 10:24:20</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Bom Jardim</t>
+          <t>Aperibé</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -517,7 +517,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>cordeiro.rj.gov.br</t>
+          <t>araruama.rj.gov.br</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -527,12 +527,12 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2025-01-23 16:23:01</t>
+          <t>2025-01-31 10:25:09</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Cordeiro</t>
+          <t>Araruama</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -544,7 +544,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>angra.rj.gov.br</t>
+          <t>areal.rj.gov.br</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -554,12 +554,12 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2025-01-29 12:40:51</t>
+          <t>2025-01-31 10:25:13</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Angra dos Reis</t>
+          <t>Areal</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -571,7 +571,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>aperibe.rj.gov.br</t>
+          <t xml:space="preserve">arraial.rj.gov.br </t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -581,12 +581,12 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2025-01-30 12:57:05</t>
+          <t>2025-01-31 10:25:25</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Aperibé</t>
+          <t>Arraial do Cabo</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -598,7 +598,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>araruama.rj.gov.br</t>
+          <t>barramansa.rj.gov.br</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -608,16 +608,24 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>2025-01-15 13:45:18</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
+          <t>2025-01-31 10:25:35</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Barra Mansa</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>areal.rj.gov.br</t>
+          <t xml:space="preserve">bomjardim.rj.gov.br </t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -627,16 +635,24 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>2025-01-15 13:45:21</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
+          <t>2025-01-31 10:25:39</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Bom Jardim</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>buzios.rj.gov.br</t>
+          <t xml:space="preserve">bomjesus.rj.gov.br </t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -646,16 +662,24 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>2025-01-15 13:45:33</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
+          <t>2025-01-31 10:25:43</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Bom Jesus do Itabapoana</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>arraial.rj.gov.br</t>
+          <t xml:space="preserve">buzios.rj.gov.br </t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -665,16 +689,24 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>2025-01-15 13:45:41</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
+          <t>2025-01-31 10:25:49</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Armação dos Búzios</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>barramansa.rj.gov.br</t>
+          <t xml:space="preserve">cabofrio.rj.gov.br </t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -684,35 +716,51 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>2025-01-15 13:47:02</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
+          <t>2025-01-31 10:25:57</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Cabo Frio</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>prefeituradebelfordroxo.rj.gov.br</t>
+          <t xml:space="preserve">cachoeirasdemacacu.rj.gov.br </t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>SUCESSO</t>
+          <t>ERRO</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>2025-01-15 13:47:08</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr"/>
-      <c r="E12" t="inlineStr"/>
+          <t>2025-01-31 10:26:05</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Cachoeiras de Macacu</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>bomjesus.rj.gov.br</t>
+          <t xml:space="preserve">campos.rj.gov.br </t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -722,16 +770,24 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>2025-01-15 13:47:20</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr"/>
-      <c r="E13" t="inlineStr"/>
+          <t>2025-01-31 10:26:06</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Campos dos Goytacazes</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>cabofrio.rj.gov.br</t>
+          <t xml:space="preserve">cantagalo.rj.gov.br </t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -741,35 +797,51 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>2025-01-15 13:47:26</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr"/>
-      <c r="E14" t="inlineStr"/>
+          <t>2025-01-31 10:26:12</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Cantagalo</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>cachoeirasdemacacu.rj.gov.br</t>
+          <t xml:space="preserve">carapebus.rj.gov.br </t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>ERRO</t>
+          <t>SUCESSO</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>2025-01-15 13:47:35</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr"/>
-      <c r="E15" t="inlineStr"/>
+          <t>2025-01-31 10:26:18</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Carapebus</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>campos.rj.gov.br</t>
+          <t xml:space="preserve">cardosomoreira.rj.gov.br </t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -779,12 +851,12 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>2025-01-30 13:21:37</t>
+          <t>2025-01-31 10:26:22</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Campos dos Goytacazes</t>
+          <t>Cardoso Moreira</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -796,7 +868,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>levygasparian.rj.gov.br</t>
+          <t xml:space="preserve">carmo.rj.gov.br </t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -806,16 +878,24 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>2025-01-15 13:47:42</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr"/>
-      <c r="E17" t="inlineStr"/>
+          <t>2025-01-31 15:36:23</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Carmo</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>carapebus.rj.gov.br</t>
+          <t xml:space="preserve">casimirodeabreu.rj.gov.br </t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -825,16 +905,24 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>2025-01-15 13:47:53</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr"/>
-      <c r="E18" t="inlineStr"/>
+          <t>2025-01-31 10:26:37</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Casimiro de Abreu</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>conceicaodemacabu.rj.gov.br</t>
+          <t xml:space="preserve">conceicaodemacabu.rj.gov.br </t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -844,16 +932,24 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>2025-01-15 13:47:57</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr"/>
-      <c r="E19" t="inlineStr"/>
+          <t>2025-01-31 15:36:39</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Conceição de Macabu</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>duquedecaxias.rj.gov.br</t>
+          <t xml:space="preserve">cordeiro.rj.gov.br </t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -863,16 +959,24 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>2025-01-15 13:48:02</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr"/>
-      <c r="E20" t="inlineStr"/>
+          <t>2025-01-31 10:26:51</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Cordeiro</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>italva.rj.gov.br</t>
+          <t xml:space="preserve">duasbarras.rj.gov.br </t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -882,16 +986,24 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>2025-01-15 13:48:16</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr"/>
-      <c r="E21" t="inlineStr"/>
+          <t>2025-01-31 10:26:58</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Duas Barras</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>itatiaia.rj.gov.br</t>
+          <t xml:space="preserve">duquedecaxias.rj.gov.br </t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -901,16 +1013,24 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>2025-01-15 13:48:22</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr"/>
-      <c r="E22" t="inlineStr"/>
+          <t>2025-01-31 10:27:03</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Duque de Caxias</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>japeri.rj.gov.br</t>
+          <t xml:space="preserve">guapimirim.rj.gov.br </t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -920,35 +1040,51 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>2025-01-15 13:48:41</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr"/>
-      <c r="E23" t="inlineStr"/>
+          <t>2025-01-31 10:27:16</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Guapimirim</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>laje.rj.gov.br</t>
+          <t xml:space="preserve">iguaba.rj.gov.br </t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>ERRO</t>
+          <t>SUCESSO</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>2025-01-15 13:48:51</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr"/>
-      <c r="E24" t="inlineStr"/>
+          <t>2025-01-31 10:27:46</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Iguaba Grande</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>macae.rj.gov.br</t>
+          <t xml:space="preserve">itaborai.rj.gov.br </t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -958,16 +1094,24 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>2025-01-15 13:49:23</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr"/>
-      <c r="E25" t="inlineStr"/>
+          <t>2025-01-31 10:27:50</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Itaboraí</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>mendes.rj.gov.br</t>
+          <t xml:space="preserve">itaguai.rj.gov.br </t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -977,16 +1121,24 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>2025-01-15 13:49:31</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr"/>
-      <c r="E26" t="inlineStr"/>
+          <t>2025-01-31 10:28:03</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Itaguaí</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>miracema.rj.gov.br</t>
+          <t xml:space="preserve">italva.rj.gov.br </t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -996,16 +1148,24 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>2025-01-15 13:49:36</t>
-        </is>
-      </c>
-      <c r="D27" t="inlineStr"/>
-      <c r="E27" t="inlineStr"/>
+          <t>2025-01-31 10:28:16</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Italva</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>miguelpereira.rj.gov.br</t>
+          <t xml:space="preserve">itaocara.rj.gov.br </t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1015,16 +1175,24 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>2025-01-15 13:50:23</t>
-        </is>
-      </c>
-      <c r="D28" t="inlineStr"/>
-      <c r="E28" t="inlineStr"/>
+          <t>2025-01-31 10:28:43</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Itaocara</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>natividade.rj.gov.br</t>
+          <t xml:space="preserve">itaperuna.rj.gov.br </t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1034,16 +1202,24 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>2025-01-15 13:50:28</t>
-        </is>
-      </c>
-      <c r="D29" t="inlineStr"/>
-      <c r="E29" t="inlineStr"/>
+          <t>2025-01-31 10:28:51</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Itaperuna</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>nilopolis.rj.gov.br</t>
+          <t xml:space="preserve">itatiaia.rj.gov.br </t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1053,16 +1229,24 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>2025-01-15 13:50:38</t>
-        </is>
-      </c>
-      <c r="D30" t="inlineStr"/>
-      <c r="E30" t="inlineStr"/>
+          <t>2025-01-31 10:29:01</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Itatiaia</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>niteroi.rj.gov.br</t>
+          <t xml:space="preserve">japeri.rj.gov.br </t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -1072,12 +1256,12 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>2025-01-30 15:33:58</t>
+          <t>2025-01-31 10:29:31</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Niterói</t>
+          <t>Japeri</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
@@ -1089,7 +1273,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>novaiguacu.rj.gov.br</t>
+          <t xml:space="preserve">laje.rj.gov.br </t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -1099,54 +1283,78 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>2025-01-15 13:51:06</t>
-        </is>
-      </c>
-      <c r="D32" t="inlineStr"/>
-      <c r="E32" t="inlineStr"/>
+          <t>2025-01-31 10:29:46</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Laje do Muriaé</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>paracambi.rj.gov.br</t>
+          <t xml:space="preserve">levygasparian.rj.gov.br </t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>ERRO</t>
+          <t>SUCESSO</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>2025-01-15 13:51:14</t>
-        </is>
-      </c>
-      <c r="D33" t="inlineStr"/>
-      <c r="E33" t="inlineStr"/>
+          <t>2025-01-31 10:29:53</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Comendador Levy Gasparian</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>paraty.rj.gov.br</t>
+          <t xml:space="preserve">macae.rj.gov.br </t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>SUCESSO</t>
+          <t>ERRO</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>2025-01-15 13:51:14</t>
-        </is>
-      </c>
-      <c r="D34" t="inlineStr"/>
-      <c r="E34" t="inlineStr"/>
+          <t>2025-01-31 10:30:05</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Macaé</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>patydoalferes.rj.gov.b</t>
+          <t xml:space="preserve">mage.rj.gov.br </t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1156,16 +1364,24 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>2025-01-15 13:51:25</t>
-        </is>
-      </c>
-      <c r="D35" t="inlineStr"/>
-      <c r="E35" t="inlineStr"/>
+          <t>2025-01-31 10:35:05</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>Magé</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>petropolis.rj.gov.br</t>
+          <t xml:space="preserve">mangaratiba.rj.gov.br </t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -1175,12 +1391,12 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>2025-01-30 14:20:13</t>
+          <t>2025-01-31 10:35:06</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Petrópolis</t>
+          <t>Mangaratiba</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
@@ -1192,7 +1408,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>pirai.rj.gov.br</t>
+          <t xml:space="preserve">marica.rj.gov.br </t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -1202,12 +1418,12 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>2025-01-30 14:20:21</t>
+          <t>2025-01-31 10:35:20</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Barra do Piraí</t>
+          <t>Maricá</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
@@ -1219,7 +1435,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>porciuncula.rj.gov.br</t>
+          <t xml:space="preserve">mendes.rj.gov.br </t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -1229,16 +1445,24 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>2025-01-15 13:51:33</t>
-        </is>
-      </c>
-      <c r="D38" t="inlineStr"/>
-      <c r="E38" t="inlineStr"/>
+          <t>2025-01-31 10:35:32</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Mendes</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>portoreal.rj.gov.br</t>
+          <t>meriti.rj.gov.br</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -1248,16 +1472,24 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>2025-01-15 13:51:38</t>
-        </is>
-      </c>
-      <c r="D39" t="inlineStr"/>
-      <c r="E39" t="inlineStr"/>
+          <t>2025-01-31 10:36:01</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>São João de Meriti</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>quatis.rj.gov.br</t>
+          <t xml:space="preserve">mesquita.rj.gov.br </t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -1267,16 +1499,24 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>2025-01-15 13:51:44</t>
-        </is>
-      </c>
-      <c r="D40" t="inlineStr"/>
-      <c r="E40" t="inlineStr"/>
+          <t>2025-01-31 10:36:09</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Mesquita</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>queimados.rj.gov.br</t>
+          <t xml:space="preserve">miguelpereira.rj.gov.br </t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -1286,16 +1526,24 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>2025-01-15 13:51:53</t>
-        </is>
-      </c>
-      <c r="D41" t="inlineStr"/>
-      <c r="E41" t="inlineStr"/>
+          <t>2025-01-31 10:36:20</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>Miguel Pereira</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>resende.rj.gov.br</t>
+          <t xml:space="preserve">miracema.rj.gov.br </t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -1305,12 +1553,12 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>2025-01-30 15:34:09</t>
+          <t>2025-01-31 10:36:25</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Resende</t>
+          <t>Miracema</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
@@ -1322,7 +1570,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>rioclaro.rj.gov.br</t>
+          <t xml:space="preserve">natividade.rj.gov.br </t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -1332,16 +1580,24 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>2025-01-15 13:52:12</t>
-        </is>
-      </c>
-      <c r="D43" t="inlineStr"/>
-      <c r="E43" t="inlineStr"/>
+          <t>2025-01-31 10:36:41</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>Natividade</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>riodasostras.rj.gov.br</t>
+          <t xml:space="preserve">nilopolis.rj.gov.br </t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -1351,20 +1607,24 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>2025-01-30 15:34:17</t>
+          <t>2025-01-31 10:36:52</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Rio das Ostras</t>
-        </is>
-      </c>
-      <c r="E44" t="inlineStr"/>
+          <t>Nilópolis</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>sapucaia.rj.gov.br</t>
+          <t xml:space="preserve">niteroi.rj.gov.br </t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -1374,16 +1634,24 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>2025-01-15 13:52:37</t>
-        </is>
-      </c>
-      <c r="D45" t="inlineStr"/>
-      <c r="E45" t="inlineStr"/>
+          <t>2025-01-31 10:37:08</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>Niterói</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>saofidelis.rj.gov.br</t>
+          <t xml:space="preserve">novafriburgo.rj.gov.br </t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -1393,16 +1661,24 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>2025-01-15 13:52:46</t>
-        </is>
-      </c>
-      <c r="D46" t="inlineStr"/>
-      <c r="E46" t="inlineStr"/>
+          <t>2025-01-31 10:37:20</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>Nova Friburgo</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>seropedica.rj.gov.br</t>
+          <t xml:space="preserve">novaiguacu.rj.gov.br </t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -1412,54 +1688,78 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>2025-01-15 13:53:16</t>
-        </is>
-      </c>
-      <c r="D47" t="inlineStr"/>
-      <c r="E47" t="inlineStr"/>
+          <t>2025-01-31 10:37:39</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>Nova Iguaçu</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>sjvriopreto.rj.gov.br</t>
+          <t xml:space="preserve">paracambi.rj.gov.br </t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>SUCESSO</t>
+          <t>ERRO</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>2025-01-15 13:53:24</t>
-        </is>
-      </c>
-      <c r="D48" t="inlineStr"/>
-      <c r="E48" t="inlineStr"/>
+          <t>2025-01-31 10:37:48</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>Paracambi</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>saosebastiao.rj.gov.br</t>
+          <t xml:space="preserve">paraibadosul.rj.gov.br </t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>ERRO</t>
+          <t>SUCESSO</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>2025-01-15 13:53:31</t>
-        </is>
-      </c>
-      <c r="D49" t="inlineStr"/>
-      <c r="E49" t="inlineStr"/>
+          <t>2025-01-31 10:37:49</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>Paraíba do Sul</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>silvajardim.rj.gov.br</t>
+          <t xml:space="preserve">paraty.rj.gov.br </t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -1469,16 +1769,24 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>2025-01-15 13:53:32</t>
-        </is>
-      </c>
-      <c r="D50" t="inlineStr"/>
-      <c r="E50" t="inlineStr"/>
+          <t>2025-01-31 10:37:59</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>Paraty</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>sumidouro.rj.gov.br</t>
+          <t xml:space="preserve">patydoalferes.rj.gov.br </t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -1488,16 +1796,24 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>2025-01-15 13:53:38</t>
-        </is>
-      </c>
-      <c r="D51" t="inlineStr"/>
-      <c r="E51" t="inlineStr"/>
+          <t>2025-01-31 10:38:08</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>Paty do Alferes</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>tangua.rj.gov.br</t>
+          <t>paulodefrontin.rj.gov.br</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -1507,16 +1823,24 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>2025-01-15 13:53:45</t>
-        </is>
-      </c>
-      <c r="D52" t="inlineStr"/>
-      <c r="E52" t="inlineStr"/>
+          <t>2025-01-31 10:38:14</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>Engenheiro Paulo de Frontin</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>teresopolis.rj.gov.br</t>
+          <t xml:space="preserve">petropolis.rj.gov.br </t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -1526,12 +1850,12 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>2025-01-30 15:34:34</t>
+          <t>2025-01-31 10:38:20</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Teresópolis</t>
+          <t>Petrópolis</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
@@ -1543,7 +1867,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>trajanodemoraes.rj.gov.br</t>
+          <t xml:space="preserve">pinheiral.rj.gov.br </t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -1553,16 +1877,24 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>2025-01-15 13:54:00</t>
-        </is>
-      </c>
-      <c r="D54" t="inlineStr"/>
-      <c r="E54" t="inlineStr"/>
+          <t>2025-01-31 10:38:33</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>Pinheiral</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>tresrios.rj.gov.br</t>
+          <t xml:space="preserve">pirai.rj.gov.br </t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -1572,16 +1904,24 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>2025-01-15 13:54:06</t>
-        </is>
-      </c>
-      <c r="D55" t="inlineStr"/>
-      <c r="E55" t="inlineStr"/>
+          <t>2025-01-31 10:39:06</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>Piraí</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>valenca.rj.gov.br</t>
+          <t>pmsfi.rj.gov.br</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -1591,12 +1931,12 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>2025-01-30 10:15:23</t>
+          <t>2025-01-31 10:39:12</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>Valencia</t>
+          <t>São Francisco de Itabapoana</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
@@ -1608,7 +1948,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>vassouras.rj.gov.br</t>
+          <t>pmsmm.rj.gov.br</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -1618,16 +1958,24 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>2025-01-15 13:54:25</t>
-        </is>
-      </c>
-      <c r="D57" t="inlineStr"/>
-      <c r="E57" t="inlineStr"/>
+          <t>2025-01-31 10:39:20</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>Santa Maria Madalena</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>voltaredonda.rj.gov.br</t>
+          <t>pmspa.rj.gov.br</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -1637,16 +1985,24 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>2025-01-15 13:54:41</t>
-        </is>
-      </c>
-      <c r="D58" t="inlineStr"/>
-      <c r="E58" t="inlineStr"/>
+          <t>2025-01-31 10:39:28</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>São Pedro da Aldeia</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro</t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>itaocara.rj.gov.br</t>
+          <t xml:space="preserve">porciuncula.rj.gov.br </t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -1656,16 +2012,24 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>2025-01-15 13:54:47</t>
-        </is>
-      </c>
-      <c r="D59" t="inlineStr"/>
-      <c r="E59" t="inlineStr"/>
+          <t>2025-01-31 10:39:35</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>Porciúncula</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>prefeituradebelfordroxo.rj.gov.br</t>
+          <t>portalbarradopirai.com.br</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -1675,16 +2039,24 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>2025-01-15 13:54:53</t>
-        </is>
-      </c>
-      <c r="D60" t="inlineStr"/>
-      <c r="E60" t="inlineStr"/>
+          <t>2025-01-31 10:39:41</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>Barra do Piraí</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>portal.prefeituradecambuci.rj.gov.br</t>
+          <t xml:space="preserve">portoreal.rj.gov.br </t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -1694,16 +2066,24 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>2025-01-15 13:54:58</t>
-        </is>
-      </c>
-      <c r="D61" t="inlineStr"/>
-      <c r="E61" t="inlineStr"/>
+          <t>2025-01-31 10:39:52</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>Porto Real</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>cantagalo.rj.gov.br</t>
+          <t xml:space="preserve">prefeituradebelfordroxo.rj.gov.br </t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -1713,16 +2093,24 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>2025-01-15 13:55:30</t>
-        </is>
-      </c>
-      <c r="D62" t="inlineStr"/>
-      <c r="E62" t="inlineStr"/>
+          <t>2025-01-31 10:40:01</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>Belford Roxo</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro</t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>cardosomoreira.rj.gov.br</t>
+          <t>prefeituradecambuci.rj.gov.br</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -1732,16 +2120,24 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>2025-01-15 13:55:35</t>
-        </is>
-      </c>
-      <c r="D63" t="inlineStr"/>
-      <c r="E63" t="inlineStr"/>
+          <t>2025-01-31 10:40:16</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>Cambuci</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro</t>
+        </is>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>carmo.rj.gov.br</t>
+          <t>prefeituramacuco.rj.gov.br</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -1751,16 +2147,24 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>2025-01-15 13:55:41</t>
-        </is>
-      </c>
-      <c r="D64" t="inlineStr"/>
-      <c r="E64" t="inlineStr"/>
+          <t>2025-01-31 10:40:25</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>Macuco</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>casimirodeabreu.rj.gov.br</t>
+          <t xml:space="preserve">quatis.rj.gov.br </t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -1770,16 +2174,24 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>2025-01-15 13:55:50</t>
-        </is>
-      </c>
-      <c r="D65" t="inlineStr"/>
-      <c r="E65" t="inlineStr"/>
+          <t>2025-01-31 10:40:36</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>Quatis</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro</t>
+        </is>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>casimirodeabreu.rj.gov.br</t>
+          <t xml:space="preserve">queimados.rj.gov.br </t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -1789,16 +2201,24 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>2025-01-15 13:55:57</t>
-        </is>
-      </c>
-      <c r="D66" t="inlineStr"/>
-      <c r="E66" t="inlineStr"/>
+          <t>2025-01-31 10:40:49</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>Queimados</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>paulodefrontin.rj.gov.br</t>
+          <t xml:space="preserve">quissama.rj.gov.br </t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -1808,16 +2228,24 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>2025-01-15 13:56:04</t>
-        </is>
-      </c>
-      <c r="D67" t="inlineStr"/>
-      <c r="E67" t="inlineStr"/>
+          <t>2025-01-31 10:40:59</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>Quissamã</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>guapimirim.rj.gov.br</t>
+          <t xml:space="preserve">resende.rj.gov.br </t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
@@ -1827,16 +2255,24 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>2025-01-15 13:56:09</t>
-        </is>
-      </c>
-      <c r="D68" t="inlineStr"/>
-      <c r="E68" t="inlineStr"/>
+          <t>2025-01-31 10:41:15</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>Resende</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro</t>
+        </is>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>iguaba.rj.gov.br</t>
+          <t xml:space="preserve">rio.rj.gov.br </t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -1846,54 +2282,78 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>2025-01-15 13:56:30</t>
-        </is>
-      </c>
-      <c r="D69" t="inlineStr"/>
-      <c r="E69" t="inlineStr"/>
+          <t>2025-01-31 10:41:29</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro</t>
+        </is>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>site.ib.itaborai.rj.gov.br</t>
+          <t xml:space="preserve">riobonito.rj.gov.br </t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>ERRO</t>
+          <t>SUCESSO</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>2025-01-15 13:56:36</t>
-        </is>
-      </c>
-      <c r="D70" t="inlineStr"/>
-      <c r="E70" t="inlineStr"/>
+          <t>2025-01-31 10:41:37</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>Rio Bonito</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro</t>
+        </is>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>novoportal.itaguai.rj.gov.br</t>
+          <t xml:space="preserve">rioclaro.rj.gov.br </t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>ERRO</t>
+          <t>SUCESSO</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>2025-01-15 13:56:36</t>
-        </is>
-      </c>
-      <c r="D71" t="inlineStr"/>
-      <c r="E71" t="inlineStr"/>
+          <t>2025-01-31 10:41:47</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>Rio Claro</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro</t>
+        </is>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>itaperuna.rj.gov.br</t>
+          <t xml:space="preserve">riodasflores.rj.gov.br </t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -1903,54 +2363,78 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>2025-01-15 13:56:37</t>
-        </is>
-      </c>
-      <c r="D72" t="inlineStr"/>
-      <c r="E72" t="inlineStr"/>
+          <t>2025-01-31 10:42:00</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>Rio das Flores</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro</t>
+        </is>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>prefeituramacuco.rj.gov.br</t>
+          <t xml:space="preserve">riodasostras.rj.gov.br </t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>SUCESSO</t>
+          <t>ERRO</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>2025-01-15 13:56:51</t>
-        </is>
-      </c>
-      <c r="D73" t="inlineStr"/>
-      <c r="E73" t="inlineStr"/>
+          <t>2025-01-31 10:42:06</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>Rio das Ostras</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro</t>
+        </is>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>mage.rj.gov.br</t>
+          <t>santoantoniodepadua.rj.gov.br</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>ERRO</t>
+          <t>SUCESSO</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>2025-01-15 13:57:03</t>
-        </is>
-      </c>
-      <c r="D74" t="inlineStr"/>
-      <c r="E74" t="inlineStr"/>
+          <t>2025-01-31 10:42:20</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>Santo Antônio de Pádua</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro</t>
+        </is>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>mangaratiba.rj.gov.br</t>
+          <t xml:space="preserve">saofidelis.rj.gov.br </t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -1960,16 +2444,24 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>2025-01-15 13:57:03</t>
-        </is>
-      </c>
-      <c r="D75" t="inlineStr"/>
-      <c r="E75" t="inlineStr"/>
+          <t>2025-01-31 10:42:34</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>São Fidélis</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro</t>
+        </is>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>marica.rj.gov.br</t>
+          <t xml:space="preserve">saogoncalo.rj.gov.br </t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -1979,16 +2471,24 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>2025-01-15 13:57:17</t>
-        </is>
-      </c>
-      <c r="D76" t="inlineStr"/>
-      <c r="E76" t="inlineStr"/>
+          <t>2025-01-31 10:44:42</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>São Gonçalo</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro</t>
+        </is>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>prefeitura.mesquita.rj.gov.br</t>
+          <t>saojosedeuba.rj.gov.br</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -1998,16 +2498,24 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>2025-01-15 13:57:47</t>
-        </is>
-      </c>
-      <c r="D77" t="inlineStr"/>
-      <c r="E77" t="inlineStr"/>
+          <t>2025-01-31 10:44:52</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>São José de Ubá</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro</t>
+        </is>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>paraibadosul.rj.gov.br</t>
+          <t xml:space="preserve">sapucaia.rj.gov.br </t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -2017,35 +2525,51 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>2025-01-15 13:58:01</t>
-        </is>
-      </c>
-      <c r="D78" t="inlineStr"/>
-      <c r="E78" t="inlineStr"/>
+          <t>2025-01-31 10:45:02</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>Sapucaia</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro</t>
+        </is>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>pinheiral.rj.gov.br</t>
+          <t xml:space="preserve">saquarema.rj.gov.br </t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>ERRO</t>
+          <t>SUCESSO</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>2025-01-15 13:58:15</t>
-        </is>
-      </c>
-      <c r="D79" t="inlineStr"/>
-      <c r="E79" t="inlineStr"/>
+          <t>2025-01-31 10:45:09</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>Saquarema</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro</t>
+        </is>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>quissama.rj.gov.br</t>
+          <t xml:space="preserve">seropedica.rj.gov.br </t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -2055,16 +2579,24 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>2025-01-15 14:00:12</t>
-        </is>
-      </c>
-      <c r="D80" t="inlineStr"/>
-      <c r="E80" t="inlineStr"/>
+          <t>2025-01-31 10:45:17</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>Seropédica</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro</t>
+        </is>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>riobonito.rj.gov.br</t>
+          <t xml:space="preserve">silvajardim.rj.gov.br </t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -2074,16 +2606,24 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>2025-01-15 14:00:28</t>
-        </is>
-      </c>
-      <c r="D81" t="inlineStr"/>
-      <c r="E81" t="inlineStr"/>
+          <t>2025-01-31 10:45:25</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>Silva Jardim</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro</t>
+        </is>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>riodasflores.rj.gov.br</t>
+          <t>sjb.rj.gov.br</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
@@ -2093,16 +2633,24 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>2025-01-15 14:00:37</t>
-        </is>
-      </c>
-      <c r="D82" t="inlineStr"/>
-      <c r="E82" t="inlineStr"/>
+          <t>2025-01-31 10:45:32</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>São João da Barra</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro</t>
+        </is>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>pmsmm.rj.gov.br</t>
+          <t xml:space="preserve">sjvriopreto.rj.gov.br </t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
@@ -2112,16 +2660,24 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>2025-01-15 14:00:45</t>
-        </is>
-      </c>
-      <c r="D83" t="inlineStr"/>
-      <c r="E83" t="inlineStr"/>
+          <t>2025-01-31 10:45:38</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>São José do Vale do Rio Preto</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro</t>
+        </is>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>santoantoniodepadua.rj.gov.br</t>
+          <t xml:space="preserve">ssalto.rj.gov.br </t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -2131,16 +2687,24 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>2025-01-15 14:01:01</t>
-        </is>
-      </c>
-      <c r="D84" t="inlineStr"/>
-      <c r="E84" t="inlineStr"/>
+          <t>2025-01-31 10:45:46</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>São Sebastião do Alto</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro</t>
+        </is>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>osaogoncalo.com.br</t>
+          <t xml:space="preserve">sumidouro.rj.gov.br </t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -2150,16 +2714,24 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>2025-01-15 14:01:13</t>
-        </is>
-      </c>
-      <c r="D85" t="inlineStr"/>
-      <c r="E85" t="inlineStr"/>
+          <t>2025-01-31 10:45:55</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>Sumidouro</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro</t>
+        </is>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>pmsfi.rj.gov.br</t>
+          <t xml:space="preserve">tangua.rj.gov.br </t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -2169,54 +2741,78 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>2025-01-15 14:01:28</t>
-        </is>
-      </c>
-      <c r="D86" t="inlineStr"/>
-      <c r="E86" t="inlineStr"/>
+          <t>2025-01-31 10:46:02</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>Tanguá</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro</t>
+        </is>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>sjb.rj.gov.b</t>
+          <t xml:space="preserve">teresopolis.rj.gov.br </t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>ERRO</t>
+          <t>SUCESSO</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>2025-01-15 14:01:37</t>
-        </is>
-      </c>
-      <c r="D87" t="inlineStr"/>
-      <c r="E87" t="inlineStr"/>
+          <t>2025-01-31 10:46:33</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>Teresópolis</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro</t>
+        </is>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>portal.meriti.rj.gov.br</t>
+          <t xml:space="preserve">trajanodemoraes.rj.gov.br </t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>ERRO</t>
+          <t>SUCESSO</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>2025-01-15 14:01:37</t>
-        </is>
-      </c>
-      <c r="D88" t="inlineStr"/>
-      <c r="E88" t="inlineStr"/>
+          <t>2025-01-31 10:46:42</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>Trajano de Moraes</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro</t>
+        </is>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>saojosedeuba.rj.gov.br</t>
+          <t xml:space="preserve">tresrios.rj.gov.br </t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -2226,16 +2822,24 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>2025-01-15 14:01:37</t>
-        </is>
-      </c>
-      <c r="D89" t="inlineStr"/>
-      <c r="E89" t="inlineStr"/>
+          <t>2025-01-31 10:46:48</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>Três Rios</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro</t>
+        </is>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>pmspa.rj.gov.br</t>
+          <t xml:space="preserve">valenca.rj.gov.br </t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
@@ -2245,16 +2849,24 @@
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>2025-01-15 14:01:45</t>
-        </is>
-      </c>
-      <c r="D90" t="inlineStr"/>
-      <c r="E90" t="inlineStr"/>
+          <t>2025-01-31 10:46:57</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>Valença</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro</t>
+        </is>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>ssalto.rj.gov.br</t>
+          <t xml:space="preserve">varresai.rj.gov.br </t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
@@ -2264,16 +2876,24 @@
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>2025-01-15 14:01:53</t>
-        </is>
-      </c>
-      <c r="D91" t="inlineStr"/>
-      <c r="E91" t="inlineStr"/>
+          <t>2025-01-31 10:47:04</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>Varre-Sai</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro</t>
+        </is>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>saquarema.rj.gov.br</t>
+          <t xml:space="preserve">vassouras.rj.gov.br </t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
@@ -2283,16 +2903,24 @@
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>2025-01-15 14:02:22</t>
-        </is>
-      </c>
-      <c r="D92" t="inlineStr"/>
-      <c r="E92" t="inlineStr"/>
+          <t>2025-01-31 10:47:10</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>Vassouras</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro</t>
+        </is>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>acrelandia.ac.gov.br</t>
+          <t>voltaredonda.rj.gov.br</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
@@ -2302,69 +2930,15 @@
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>2025-01-23 16:23:08</t>
+          <t>2025-01-31 10:47:27</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>Acrelândia</t>
+          <t>Volta Redonda</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
-        <is>
-          <t>Acre</t>
-        </is>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" t="inlineStr">
-        <is>
-          <t>assisbrasil.ac.gov.br</t>
-        </is>
-      </c>
-      <c r="B94" t="inlineStr">
-        <is>
-          <t>ERRO</t>
-        </is>
-      </c>
-      <c r="C94" t="inlineStr">
-        <is>
-          <t>2025-01-23 16:23:14</t>
-        </is>
-      </c>
-      <c r="D94" t="inlineStr">
-        <is>
-          <t>Assis Brasil</t>
-        </is>
-      </c>
-      <c r="E94" t="inlineStr">
-        <is>
-          <t>Acre</t>
-        </is>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" t="inlineStr">
-        <is>
-          <t>prefeitura.rio</t>
-        </is>
-      </c>
-      <c r="B95" t="inlineStr">
-        <is>
-          <t>SUCESSO</t>
-        </is>
-      </c>
-      <c r="C95" t="inlineStr">
-        <is>
-          <t>2025-01-30 13:36:07</t>
-        </is>
-      </c>
-      <c r="D95" t="inlineStr">
-        <is>
-          <t>Rio de Janeiro</t>
-        </is>
-      </c>
-      <c r="E95" t="inlineStr">
         <is>
           <t>Rio de Janeiro</t>
         </is>

</xml_diff>

<commit_message>
bot 2 com prints para depuracao
</commit_message>
<xml_diff>
--- a/Bot-Varredura/dominios.xlsx
+++ b/Bot-Varredura/dominios.xlsx
@@ -473,7 +473,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2025-01-31 10:24:15</t>
+          <t>2025-02-02 20:00:31</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -500,7 +500,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2025-01-31 10:24:20</t>
+          <t>2025-02-02 20:00:41</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -527,7 +527,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2025-01-31 10:25:09</t>
+          <t>2025-02-02 20:01:29</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -554,7 +554,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2025-01-31 10:25:13</t>
+          <t>2025-02-02 20:01:34</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -581,7 +581,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2025-01-31 10:25:25</t>
+          <t>2025-02-02 20:01:47</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -608,7 +608,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>2025-01-31 10:25:35</t>
+          <t>2025-02-02 20:02:12</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -635,7 +635,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>2025-01-31 10:25:39</t>
+          <t>2025-02-02 20:02:17</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -662,7 +662,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>2025-01-31 10:25:43</t>
+          <t>2025-02-02 20:02:25</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -689,7 +689,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>2025-01-31 10:25:49</t>
+          <t>2025-02-02 20:02:31</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -716,7 +716,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>2025-01-31 10:25:57</t>
+          <t>2025-02-02 20:02:41</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -743,7 +743,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>2025-01-31 10:26:05</t>
+          <t>2025-02-02 20:02:50</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -770,7 +770,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>2025-01-31 10:26:06</t>
+          <t>2025-02-03 00:02:47</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -797,7 +797,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>2025-01-31 10:26:12</t>
+          <t>2025-02-03 00:02:54</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -824,7 +824,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>2025-01-31 10:26:18</t>
+          <t>2025-02-03 00:03:00</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -851,7 +851,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>2025-01-31 10:26:22</t>
+          <t>2025-02-03 00:03:05</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -878,7 +878,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>2025-01-31 15:36:23</t>
+          <t>2025-02-03 00:03:12</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -905,7 +905,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>2025-01-31 10:26:37</t>
+          <t>2025-02-03 00:03:24</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -932,7 +932,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>2025-01-31 15:36:39</t>
+          <t>2025-02-03 00:03:32</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -959,7 +959,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>2025-01-31 10:26:51</t>
+          <t>2025-02-03 00:03:38</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -1904,7 +1904,7 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>2025-01-31 10:39:06</t>
+          <t>2025-02-02 22:30:23</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
@@ -1931,7 +1931,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>2025-01-31 10:39:12</t>
+          <t>2025-02-02 22:30:28</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -1958,7 +1958,7 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>2025-01-31 10:39:20</t>
+          <t>2025-02-02 22:30:37</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
@@ -1985,7 +1985,7 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>2025-01-31 10:39:28</t>
+          <t>2025-02-02 22:30:45</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
@@ -2012,7 +2012,7 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>2025-01-31 10:39:35</t>
+          <t>2025-02-02 22:30:53</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
@@ -2039,7 +2039,7 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>2025-01-31 10:39:41</t>
+          <t>2025-02-02 22:30:58</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -2066,7 +2066,7 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>2025-01-31 10:39:52</t>
+          <t>2025-02-02 22:31:11</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -2093,7 +2093,7 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>2025-01-31 10:40:01</t>
+          <t>2025-02-02 22:31:17</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
@@ -2120,7 +2120,7 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>2025-01-31 10:40:16</t>
+          <t>2025-02-02 22:31:34</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
@@ -2147,7 +2147,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>2025-01-31 10:40:25</t>
+          <t>2025-02-02 22:31:44</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
@@ -2174,7 +2174,7 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>2025-01-31 10:40:36</t>
+          <t>2025-02-02 22:31:58</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
@@ -2201,7 +2201,7 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>2025-01-31 10:40:49</t>
+          <t>2025-02-02 22:32:09</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
@@ -2228,7 +2228,7 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>2025-01-31 10:40:59</t>
+          <t>2025-02-02 22:32:17</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -2255,7 +2255,7 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>2025-01-31 10:41:15</t>
+          <t>2025-02-02 22:32:34</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
@@ -2282,7 +2282,7 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>2025-01-31 10:41:29</t>
+          <t>2025-02-02 22:32:47</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
@@ -2309,7 +2309,7 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>2025-01-31 10:41:37</t>
+          <t>2025-02-02 22:32:54</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
@@ -2336,7 +2336,7 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>2025-01-31 10:41:47</t>
+          <t>2025-02-02 22:33:03</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
@@ -2363,7 +2363,7 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>2025-01-31 10:42:00</t>
+          <t>2025-02-02 22:33:16</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
@@ -2385,12 +2385,12 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>ERRO</t>
+          <t>SUCESSO</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>2025-01-31 10:42:06</t>
+          <t>2025-02-02 22:33:22</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
@@ -2417,7 +2417,7 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>2025-01-31 10:42:20</t>
+          <t>2025-02-02 22:33:44</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
@@ -2444,7 +2444,7 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>2025-01-31 10:42:34</t>
+          <t>2025-02-02 22:33:53</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
@@ -2471,7 +2471,7 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>2025-01-31 10:44:42</t>
+          <t>2025-02-02 22:34:25</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
@@ -2498,7 +2498,7 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>2025-01-31 10:44:52</t>
+          <t>2025-02-02 22:34:34</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
@@ -2525,7 +2525,7 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>2025-01-31 10:45:02</t>
+          <t>2025-02-02 22:34:40</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
@@ -2552,7 +2552,7 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>2025-01-31 10:45:09</t>
+          <t>2025-02-02 22:34:48</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
@@ -2579,7 +2579,7 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>2025-01-31 10:45:17</t>
+          <t>2025-02-02 22:34:55</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
@@ -2606,7 +2606,7 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>2025-01-31 10:45:25</t>
+          <t>2025-02-02 22:35:04</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
@@ -2633,7 +2633,7 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>2025-01-31 10:45:32</t>
+          <t>2025-02-02 22:35:11</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
@@ -2660,7 +2660,7 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>2025-01-31 10:45:38</t>
+          <t>2025-02-02 22:35:15</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
@@ -2687,7 +2687,7 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>2025-01-31 10:45:46</t>
+          <t>2025-02-02 22:35:28</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
@@ -2714,7 +2714,7 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>2025-01-31 10:45:55</t>
+          <t>2025-02-02 22:35:36</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
@@ -2741,7 +2741,7 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>2025-01-31 10:46:02</t>
+          <t>2025-02-02 22:35:41</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
@@ -2768,7 +2768,7 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>2025-01-31 10:46:33</t>
+          <t>2025-02-02 22:36:52</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
@@ -2795,7 +2795,7 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>2025-01-31 10:46:42</t>
+          <t>2025-02-02 22:37:01</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
@@ -2822,7 +2822,7 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>2025-01-31 10:46:48</t>
+          <t>2025-02-02 22:37:07</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
@@ -2849,7 +2849,7 @@
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>2025-01-31 10:46:57</t>
+          <t>2025-02-02 22:37:16</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
@@ -2876,7 +2876,7 @@
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>2025-01-31 10:47:04</t>
+          <t>2025-02-02 22:37:24</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
@@ -2898,12 +2898,12 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>SUCESSO</t>
+          <t>ERRO</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>2025-01-31 10:47:10</t>
+          <t>2025-02-02 22:37:31</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
@@ -2930,7 +2930,7 @@
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>2025-01-31 10:47:27</t>
+          <t>2025-02-02 22:37:55</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">

</xml_diff>

<commit_message>
tratando erro de buzios
</commit_message>
<xml_diff>
--- a/Bot-Varredura/dominios.xlsx
+++ b/Bot-Varredura/dominios.xlsx
@@ -473,7 +473,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2025-02-02 20:00:31</t>
+          <t>2025-02-03 09:47:31</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -500,7 +500,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2025-02-02 20:00:41</t>
+          <t>2025-02-03 09:47:42</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -527,7 +527,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2025-02-02 20:01:29</t>
+          <t>2025-02-03 09:48:29</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -554,7 +554,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2025-02-02 20:01:34</t>
+          <t>2025-02-03 09:48:33</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -581,7 +581,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2025-02-02 20:01:47</t>
+          <t>2025-02-03 09:48:45</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -608,7 +608,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>2025-02-02 20:02:12</t>
+          <t>2025-02-03 09:49:27</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -635,7 +635,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>2025-02-02 20:02:17</t>
+          <t>2025-02-03 09:49:33</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -662,7 +662,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>2025-02-02 20:02:25</t>
+          <t>2025-02-03 09:49:43</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -689,7 +689,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>2025-02-02 20:02:31</t>
+          <t>2025-02-03 09:49:50</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -716,7 +716,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>2025-02-02 20:02:41</t>
+          <t>2025-02-03 09:50:06</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -743,7 +743,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>2025-02-02 20:02:50</t>
+          <t>2025-02-03 09:50:14</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -770,7 +770,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>2025-02-03 00:02:47</t>
+          <t>2025-02-03 09:50:16</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -797,7 +797,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>2025-02-03 00:02:54</t>
+          <t>2025-02-03 09:50:24</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -824,7 +824,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>2025-02-03 00:03:00</t>
+          <t>2025-02-03 09:50:29</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -851,7 +851,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>2025-02-03 00:03:05</t>
+          <t>2025-02-03 09:50:35</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -878,7 +878,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>2025-02-03 00:03:12</t>
+          <t>2025-02-03 09:50:44</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -905,7 +905,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>2025-02-03 00:03:24</t>
+          <t>2025-02-03 09:51:00</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -932,7 +932,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>2025-02-03 00:03:32</t>
+          <t>2025-02-03 09:51:09</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -959,7 +959,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>2025-02-03 00:03:38</t>
+          <t>2025-02-03 09:51:14</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -986,7 +986,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>2025-01-31 10:26:58</t>
+          <t>2025-02-03 09:51:22</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -1013,7 +1013,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>2025-01-31 10:27:03</t>
+          <t>2025-02-03 09:51:27</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -1035,12 +1035,12 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>SUCESSO</t>
+          <t>ERRO</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>2025-01-31 10:27:16</t>
+          <t>2025-02-03 09:51:40</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -1067,7 +1067,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>2025-01-31 10:27:46</t>
+          <t>2025-02-03 09:52:16</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -1094,7 +1094,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>2025-01-31 10:27:50</t>
+          <t>2025-02-03 09:52:22</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -1121,7 +1121,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>2025-01-31 10:28:03</t>
+          <t>2025-02-03 09:52:36</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -1148,7 +1148,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>2025-01-31 10:28:16</t>
+          <t>2025-02-03 09:52:53</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -1175,7 +1175,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>2025-01-31 10:28:43</t>
+          <t>2025-02-03 09:53:01</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -1202,7 +1202,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>2025-01-31 10:28:51</t>
+          <t>2025-02-03 09:53:08</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -1229,7 +1229,7 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>2025-01-31 10:29:01</t>
+          <t>2025-02-03 09:53:17</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -1256,7 +1256,7 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>2025-01-31 10:29:31</t>
+          <t>2025-02-03 09:53:46</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -1283,7 +1283,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>2025-01-31 10:29:46</t>
+          <t>2025-02-03 09:54:00</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -1310,7 +1310,7 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>2025-01-31 10:29:53</t>
+          <t>2025-02-03 09:54:16</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -1332,12 +1332,12 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>ERRO</t>
+          <t>SUCESSO</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>2025-01-31 10:30:05</t>
+          <t>2025-02-03 09:54:35</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -1364,7 +1364,7 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>2025-01-31 10:35:05</t>
+          <t>2025-02-03 09:54:46</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -1391,7 +1391,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>2025-01-31 10:35:06</t>
+          <t>2025-02-03 09:54:47</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -1418,7 +1418,7 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>2025-01-31 10:35:20</t>
+          <t>2025-02-03 09:54:57</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -1440,12 +1440,12 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>SUCESSO</t>
+          <t>ERRO</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>2025-01-31 10:35:32</t>
+          <t>2025-02-03 09:55:09</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -1472,7 +1472,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>2025-01-31 10:36:01</t>
+          <t>2025-02-03 09:55:41</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -1499,7 +1499,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>2025-01-31 10:36:09</t>
+          <t>2025-02-03 09:55:51</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -1526,7 +1526,7 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>2025-01-31 10:36:20</t>
+          <t>2025-02-03 09:56:04</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -1553,7 +1553,7 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>2025-01-31 10:36:25</t>
+          <t>2025-02-03 09:56:10</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -1580,7 +1580,7 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>2025-01-31 10:36:41</t>
+          <t>2025-02-03 09:56:58</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -1607,7 +1607,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>2025-01-31 10:36:52</t>
+          <t>2025-02-03 09:57:09</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -1634,7 +1634,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>2025-01-31 10:37:08</t>
+          <t>2025-02-03 09:57:52</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -1661,7 +1661,7 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>2025-01-31 10:37:20</t>
+          <t>2025-02-03 09:58:08</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -1688,7 +1688,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>2025-01-31 10:37:39</t>
+          <t>2025-02-03 09:58:23</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">

</xml_diff>

<commit_message>
ajuste no bot 1
</commit_message>
<xml_diff>
--- a/Bot-Varredura/dominios.xlsx
+++ b/Bot-Varredura/dominios.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Alessandro\TCC\Resende_Virmond_2025\Bot-Varredura\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\repo\pessoal\TCC\lab_redes\Resende_Virmond_2025\Bot-Varredura\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE794B34-B0D2-4124-8E1C-EC52E36C3B31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{815CEABB-73FD-4284-9E39-711A77543368}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20610" yWindow="1320" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="280">
   <si>
     <t>DOMINIO</t>
   </si>
@@ -88,7 +88,7 @@
     <t>barramansa.rj.gov.br</t>
   </si>
   <si>
-    <t>2025-02-03 09:49:27</t>
+    <t>2025-02-04 09:52:03</t>
   </si>
   <si>
     <t>Barra Mansa</t>
@@ -115,7 +115,7 @@
     <t xml:space="preserve">buzios.rj.gov.br </t>
   </si>
   <si>
-    <t>2025-02-03 09:49:50</t>
+    <t>2025-02-04 10:13:54</t>
   </si>
   <si>
     <t>Armação dos Búzios</t>
@@ -133,7 +133,7 @@
     <t xml:space="preserve">cachoeirasdemacacu.rj.gov.br </t>
   </si>
   <si>
-    <t>2025-02-03 09:50:14</t>
+    <t>2025-02-04 10:40:27</t>
   </si>
   <si>
     <t>Cachoeiras de Macacu</t>
@@ -178,7 +178,7 @@
     <t xml:space="preserve">carmo.rj.gov.br </t>
   </si>
   <si>
-    <t>2025-02-03 09:50:44</t>
+    <t>2025-02-04 10:18:33</t>
   </si>
   <si>
     <t>Carmo</t>
@@ -214,7 +214,7 @@
     <t xml:space="preserve">duasbarras.rj.gov.br </t>
   </si>
   <si>
-    <t>2025-02-03 09:51:22</t>
+    <t>2025-02-04 10:41:41</t>
   </si>
   <si>
     <t>Duas Barras</t>
@@ -223,7 +223,7 @@
     <t xml:space="preserve">duquedecaxias.rj.gov.br </t>
   </si>
   <si>
-    <t>2025-02-03 09:51:27</t>
+    <t>2025-02-04 10:42:49</t>
   </si>
   <si>
     <t>Duque de Caxias</t>
@@ -232,9 +232,6 @@
     <t xml:space="preserve">guapimirim.rj.gov.br </t>
   </si>
   <si>
-    <t>2025-02-03 09:51:40</t>
-  </si>
-  <si>
     <t>Guapimirim</t>
   </si>
   <si>
@@ -340,7 +337,7 @@
     <t xml:space="preserve">mage.rj.gov.br </t>
   </si>
   <si>
-    <t>2025-02-03 09:54:46</t>
+    <t>2025-02-04 10:43:01</t>
   </si>
   <si>
     <t>Magé</t>
@@ -457,7 +454,7 @@
     <t xml:space="preserve">paracambi.rj.gov.br </t>
   </si>
   <si>
-    <t>2025-01-31 10:37:48</t>
+    <t>2025-02-04 10:43:02</t>
   </si>
   <si>
     <t>Paracambi</t>
@@ -760,7 +757,7 @@
     <t>sjb.rj.gov.br</t>
   </si>
   <si>
-    <t>2025-02-02 22:35:11</t>
+    <t>2025-02-04 10:43:04</t>
   </si>
   <si>
     <t>São João da Barra</t>
@@ -869,6 +866,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -918,11 +918,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1228,18 +1229,16 @@
   <dimension ref="A1:E93"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="40.85546875" customWidth="1"/>
-    <col min="2" max="2" width="39.7109375" customWidth="1"/>
-    <col min="3" max="3" width="26.28515625" customWidth="1"/>
-    <col min="4" max="4" width="35.7109375" customWidth="1"/>
+    <col min="1" max="1" width="24.54296875" customWidth="1"/>
+    <col min="2" max="2" width="48.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1256,7 +1255,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1270,7 +1269,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1284,7 +1283,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -1298,7 +1297,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -1312,7 +1311,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -1326,7 +1325,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -1340,7 +1339,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -1354,7 +1353,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -1368,7 +1367,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>30</v>
       </c>
@@ -1382,7 +1381,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>33</v>
       </c>
@@ -1396,7 +1395,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>36</v>
       </c>
@@ -1410,7 +1409,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>39</v>
       </c>
@@ -1424,7 +1423,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>42</v>
       </c>
@@ -1438,7 +1437,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>45</v>
       </c>
@@ -1452,7 +1451,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>48</v>
       </c>
@@ -1466,7 +1465,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>51</v>
       </c>
@@ -1480,7 +1479,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>54</v>
       </c>
@@ -1494,7 +1493,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>57</v>
       </c>
@@ -1508,7 +1507,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>60</v>
       </c>
@@ -1522,7 +1521,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>63</v>
       </c>
@@ -1536,7 +1535,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>66</v>
       </c>
@@ -1550,995 +1549,995 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>69</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="2">
+        <v>45691.410879629628</v>
+      </c>
+      <c r="D23" t="s">
         <v>70</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
         <v>71</v>
       </c>
-      <c r="E23" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="C24" t="s">
         <v>72</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>73</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
         <v>74</v>
       </c>
-      <c r="E24" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="C25" t="s">
         <v>75</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>76</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
         <v>77</v>
       </c>
-      <c r="E25" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="C26" t="s">
         <v>78</v>
       </c>
-      <c r="C26" t="s">
+      <c r="D26" t="s">
         <v>79</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
         <v>80</v>
       </c>
-      <c r="E26" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="C27" t="s">
         <v>81</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>82</v>
       </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
         <v>83</v>
       </c>
-      <c r="E27" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="C28" t="s">
         <v>84</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
         <v>85</v>
       </c>
-      <c r="D28" t="s">
+      <c r="E28" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
         <v>86</v>
       </c>
-      <c r="E28" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="C29" t="s">
         <v>87</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
         <v>88</v>
       </c>
-      <c r="D29" t="s">
+      <c r="E29" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
         <v>89</v>
       </c>
-      <c r="E29" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="C30" t="s">
         <v>90</v>
       </c>
-      <c r="C30" t="s">
+      <c r="D30" t="s">
         <v>91</v>
       </c>
-      <c r="D30" t="s">
+      <c r="E30" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
         <v>92</v>
       </c>
-      <c r="E30" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="C31" t="s">
         <v>93</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D31" t="s">
         <v>94</v>
       </c>
-      <c r="D31" t="s">
+      <c r="E31" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
         <v>95</v>
       </c>
-      <c r="E31" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="C32" t="s">
         <v>96</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>97</v>
       </c>
-      <c r="D32" t="s">
+      <c r="E32" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
         <v>98</v>
       </c>
-      <c r="E32" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="C33" t="s">
         <v>99</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D33" t="s">
         <v>100</v>
       </c>
-      <c r="D33" t="s">
+      <c r="E33" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
         <v>101</v>
       </c>
-      <c r="E33" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="C34" t="s">
         <v>102</v>
       </c>
-      <c r="C34" t="s">
+      <c r="D34" t="s">
         <v>103</v>
       </c>
-      <c r="D34" t="s">
+      <c r="E34" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
         <v>104</v>
       </c>
-      <c r="E34" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="C35" t="s">
         <v>105</v>
       </c>
-      <c r="C35" t="s">
+      <c r="D35" t="s">
         <v>106</v>
       </c>
-      <c r="D35" t="s">
+      <c r="E35" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
         <v>107</v>
       </c>
-      <c r="E35" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="C36" t="s">
         <v>108</v>
       </c>
-      <c r="C36" t="s">
+      <c r="D36" t="s">
         <v>109</v>
       </c>
-      <c r="D36" t="s">
+      <c r="E36" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
         <v>110</v>
       </c>
-      <c r="E36" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="C37" t="s">
         <v>111</v>
       </c>
-      <c r="C37" t="s">
+      <c r="D37" t="s">
         <v>112</v>
       </c>
-      <c r="D37" t="s">
+      <c r="E37" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
         <v>113</v>
       </c>
-      <c r="E37" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="C38" t="s">
         <v>114</v>
       </c>
-      <c r="C38" t="s">
+      <c r="D38" t="s">
         <v>115</v>
       </c>
-      <c r="D38" t="s">
+      <c r="E38" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
         <v>116</v>
       </c>
-      <c r="E38" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="C39" t="s">
         <v>117</v>
       </c>
-      <c r="C39" t="s">
+      <c r="D39" t="s">
         <v>118</v>
       </c>
-      <c r="D39" t="s">
+      <c r="E39" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
         <v>119</v>
       </c>
-      <c r="E39" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+      <c r="C40" t="s">
         <v>120</v>
       </c>
-      <c r="C40" t="s">
+      <c r="D40" t="s">
         <v>121</v>
       </c>
-      <c r="D40" t="s">
+      <c r="E40" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
         <v>122</v>
       </c>
-      <c r="E40" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="C41" t="s">
         <v>123</v>
       </c>
-      <c r="C41" t="s">
+      <c r="D41" t="s">
         <v>124</v>
       </c>
-      <c r="D41" t="s">
+      <c r="E41" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
         <v>125</v>
       </c>
-      <c r="E41" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+      <c r="C42" t="s">
         <v>126</v>
       </c>
-      <c r="C42" t="s">
+      <c r="D42" t="s">
         <v>127</v>
       </c>
-      <c r="D42" t="s">
+      <c r="E42" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
         <v>128</v>
       </c>
-      <c r="E42" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+      <c r="C43" t="s">
         <v>129</v>
       </c>
-      <c r="C43" t="s">
+      <c r="D43" t="s">
         <v>130</v>
       </c>
-      <c r="D43" t="s">
+      <c r="E43" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
         <v>131</v>
       </c>
-      <c r="E43" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+      <c r="C44" t="s">
         <v>132</v>
       </c>
-      <c r="C44" t="s">
+      <c r="D44" t="s">
         <v>133</v>
       </c>
-      <c r="D44" t="s">
+      <c r="E44" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
         <v>134</v>
       </c>
-      <c r="E44" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+      <c r="C45" t="s">
         <v>135</v>
       </c>
-      <c r="C45" t="s">
+      <c r="D45" t="s">
         <v>136</v>
       </c>
-      <c r="D45" t="s">
+      <c r="E45" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
         <v>137</v>
       </c>
-      <c r="E45" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+      <c r="C46" t="s">
         <v>138</v>
       </c>
-      <c r="C46" t="s">
+      <c r="D46" t="s">
         <v>139</v>
       </c>
-      <c r="D46" t="s">
+      <c r="E46" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
         <v>140</v>
       </c>
-      <c r="E46" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+      <c r="C47" t="s">
         <v>141</v>
       </c>
-      <c r="C47" t="s">
+      <c r="D47" t="s">
         <v>142</v>
       </c>
-      <c r="D47" t="s">
+      <c r="E47" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
         <v>143</v>
       </c>
-      <c r="E47" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+      <c r="C48" t="s">
         <v>144</v>
       </c>
-      <c r="C48" t="s">
+      <c r="D48" t="s">
         <v>145</v>
       </c>
-      <c r="D48" t="s">
+      <c r="E48" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
         <v>146</v>
       </c>
-      <c r="E48" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+      <c r="C49" t="s">
         <v>147</v>
       </c>
-      <c r="C49" t="s">
+      <c r="D49" t="s">
         <v>148</v>
       </c>
-      <c r="D49" t="s">
+      <c r="E49" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
         <v>149</v>
       </c>
-      <c r="E49" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+      <c r="C50" t="s">
         <v>150</v>
       </c>
-      <c r="C50" t="s">
+      <c r="D50" t="s">
         <v>151</v>
       </c>
-      <c r="D50" t="s">
+      <c r="E50" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
         <v>152</v>
       </c>
-      <c r="E50" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+      <c r="C51" t="s">
         <v>153</v>
       </c>
-      <c r="C51" t="s">
+      <c r="D51" t="s">
         <v>154</v>
       </c>
-      <c r="D51" t="s">
+      <c r="E51" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
         <v>155</v>
       </c>
-      <c r="E51" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+      <c r="C52" t="s">
         <v>156</v>
       </c>
-      <c r="C52" t="s">
+      <c r="D52" t="s">
         <v>157</v>
       </c>
-      <c r="D52" t="s">
+      <c r="E52" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
         <v>158</v>
       </c>
-      <c r="E52" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+      <c r="C53" t="s">
         <v>159</v>
       </c>
-      <c r="C53" t="s">
+      <c r="D53" t="s">
         <v>160</v>
       </c>
-      <c r="D53" t="s">
+      <c r="E53" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
         <v>161</v>
       </c>
-      <c r="E53" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+      <c r="C54" t="s">
         <v>162</v>
       </c>
-      <c r="C54" t="s">
+      <c r="D54" t="s">
         <v>163</v>
       </c>
-      <c r="D54" t="s">
+      <c r="E54" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
         <v>164</v>
       </c>
-      <c r="E54" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+      <c r="C55" t="s">
         <v>165</v>
       </c>
-      <c r="C55" t="s">
+      <c r="D55" t="s">
         <v>166</v>
       </c>
-      <c r="D55" t="s">
+      <c r="E55" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
         <v>167</v>
       </c>
-      <c r="E55" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+      <c r="C56" t="s">
         <v>168</v>
       </c>
-      <c r="C56" t="s">
+      <c r="D56" t="s">
         <v>169</v>
       </c>
-      <c r="D56" t="s">
+      <c r="E56" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
         <v>170</v>
       </c>
-      <c r="E56" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+      <c r="C57" t="s">
         <v>171</v>
       </c>
-      <c r="C57" t="s">
+      <c r="D57" t="s">
         <v>172</v>
       </c>
-      <c r="D57" t="s">
+      <c r="E57" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
         <v>173</v>
       </c>
-      <c r="E57" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
+      <c r="C58" t="s">
         <v>174</v>
       </c>
-      <c r="C58" t="s">
+      <c r="D58" t="s">
         <v>175</v>
       </c>
-      <c r="D58" t="s">
+      <c r="E58" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
         <v>176</v>
       </c>
-      <c r="E58" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+      <c r="C59" t="s">
         <v>177</v>
       </c>
-      <c r="C59" t="s">
+      <c r="D59" t="s">
         <v>178</v>
       </c>
-      <c r="D59" t="s">
+      <c r="E59" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
         <v>179</v>
       </c>
-      <c r="E59" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
+      <c r="C60" t="s">
         <v>180</v>
       </c>
-      <c r="C60" t="s">
+      <c r="D60" t="s">
         <v>181</v>
       </c>
-      <c r="D60" t="s">
+      <c r="E60" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
         <v>182</v>
       </c>
-      <c r="E60" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
+      <c r="C61" t="s">
         <v>183</v>
       </c>
-      <c r="C61" t="s">
+      <c r="D61" t="s">
         <v>184</v>
       </c>
-      <c r="D61" t="s">
+      <c r="E61" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
         <v>185</v>
       </c>
-      <c r="E61" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
+      <c r="C62" t="s">
         <v>186</v>
       </c>
-      <c r="C62" t="s">
+      <c r="D62" t="s">
         <v>187</v>
       </c>
-      <c r="D62" t="s">
+      <c r="E62" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
         <v>188</v>
       </c>
-      <c r="E62" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
+      <c r="C63" t="s">
         <v>189</v>
       </c>
-      <c r="C63" t="s">
+      <c r="D63" t="s">
         <v>190</v>
       </c>
-      <c r="D63" t="s">
+      <c r="E63" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
         <v>191</v>
       </c>
-      <c r="E63" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
+      <c r="C64" t="s">
         <v>192</v>
       </c>
-      <c r="C64" t="s">
+      <c r="D64" t="s">
         <v>193</v>
       </c>
-      <c r="D64" t="s">
+      <c r="E64" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
         <v>194</v>
       </c>
-      <c r="E64" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
+      <c r="C65" t="s">
         <v>195</v>
       </c>
-      <c r="C65" t="s">
+      <c r="D65" t="s">
         <v>196</v>
       </c>
-      <c r="D65" t="s">
+      <c r="E65" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
         <v>197</v>
       </c>
-      <c r="E65" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
+      <c r="C66" t="s">
         <v>198</v>
       </c>
-      <c r="C66" t="s">
+      <c r="D66" t="s">
         <v>199</v>
       </c>
-      <c r="D66" t="s">
+      <c r="E66" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
         <v>200</v>
       </c>
-      <c r="E66" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
+      <c r="C67" t="s">
         <v>201</v>
       </c>
-      <c r="C67" t="s">
+      <c r="D67" t="s">
         <v>202</v>
       </c>
-      <c r="D67" t="s">
+      <c r="E67" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
         <v>203</v>
       </c>
-      <c r="E67" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
+      <c r="C68" t="s">
         <v>204</v>
       </c>
-      <c r="C68" t="s">
+      <c r="D68" t="s">
         <v>205</v>
       </c>
-      <c r="D68" t="s">
+      <c r="E68" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
         <v>206</v>
       </c>
-      <c r="E68" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
+      <c r="C69" t="s">
         <v>207</v>
       </c>
-      <c r="C69" t="s">
+      <c r="D69" t="s">
+        <v>8</v>
+      </c>
+      <c r="E69" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
         <v>208</v>
       </c>
-      <c r="D69" t="s">
-        <v>8</v>
-      </c>
-      <c r="E69" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
+      <c r="C70" t="s">
         <v>209</v>
       </c>
-      <c r="C70" t="s">
+      <c r="D70" t="s">
         <v>210</v>
       </c>
-      <c r="D70" t="s">
+      <c r="E70" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
         <v>211</v>
       </c>
-      <c r="E70" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
+      <c r="C71" t="s">
         <v>212</v>
       </c>
-      <c r="C71" t="s">
+      <c r="D71" t="s">
         <v>213</v>
       </c>
-      <c r="D71" t="s">
+      <c r="E71" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
         <v>214</v>
       </c>
-      <c r="E71" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
+      <c r="C72" t="s">
         <v>215</v>
       </c>
-      <c r="C72" t="s">
+      <c r="D72" t="s">
         <v>216</v>
       </c>
-      <c r="D72" t="s">
+      <c r="E72" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
         <v>217</v>
       </c>
-      <c r="E72" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
+      <c r="C73" t="s">
         <v>218</v>
       </c>
-      <c r="C73" t="s">
+      <c r="D73" t="s">
         <v>219</v>
       </c>
-      <c r="D73" t="s">
+      <c r="E73" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A74" t="s">
         <v>220</v>
       </c>
-      <c r="E73" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
+      <c r="C74" t="s">
         <v>221</v>
       </c>
-      <c r="C74" t="s">
+      <c r="D74" t="s">
         <v>222</v>
       </c>
-      <c r="D74" t="s">
+      <c r="E74" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A75" t="s">
         <v>223</v>
       </c>
-      <c r="E74" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
+      <c r="C75" t="s">
         <v>224</v>
       </c>
-      <c r="C75" t="s">
+      <c r="D75" t="s">
         <v>225</v>
       </c>
-      <c r="D75" t="s">
+      <c r="E75" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A76" t="s">
         <v>226</v>
       </c>
-      <c r="E75" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
+      <c r="C76" t="s">
         <v>227</v>
       </c>
-      <c r="C76" t="s">
+      <c r="D76" t="s">
         <v>228</v>
       </c>
-      <c r="D76" t="s">
+      <c r="E76" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A77" t="s">
         <v>229</v>
       </c>
-      <c r="E76" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
+      <c r="C77" t="s">
         <v>230</v>
       </c>
-      <c r="C77" t="s">
+      <c r="D77" t="s">
         <v>231</v>
       </c>
-      <c r="D77" t="s">
+      <c r="E77" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A78" t="s">
         <v>232</v>
       </c>
-      <c r="E77" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
+      <c r="C78" t="s">
         <v>233</v>
       </c>
-      <c r="C78" t="s">
+      <c r="D78" t="s">
         <v>234</v>
       </c>
-      <c r="D78" t="s">
+      <c r="E78" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A79" t="s">
         <v>235</v>
       </c>
-      <c r="E78" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
+      <c r="C79" t="s">
         <v>236</v>
       </c>
-      <c r="C79" t="s">
+      <c r="D79" t="s">
         <v>237</v>
       </c>
-      <c r="D79" t="s">
+      <c r="E79" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A80" t="s">
         <v>238</v>
       </c>
-      <c r="E79" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
+      <c r="C80" t="s">
         <v>239</v>
       </c>
-      <c r="C80" t="s">
+      <c r="D80" t="s">
         <v>240</v>
       </c>
-      <c r="D80" t="s">
+      <c r="E80" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A81" t="s">
         <v>241</v>
       </c>
-      <c r="E80" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
+      <c r="C81" t="s">
         <v>242</v>
       </c>
-      <c r="C81" t="s">
+      <c r="D81" t="s">
         <v>243</v>
       </c>
-      <c r="D81" t="s">
+      <c r="E81" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A82" t="s">
         <v>244</v>
       </c>
-      <c r="E81" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
+      <c r="C82" t="s">
         <v>245</v>
       </c>
-      <c r="C82" t="s">
+      <c r="D82" t="s">
         <v>246</v>
       </c>
-      <c r="D82" t="s">
+      <c r="E82" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
         <v>247</v>
       </c>
-      <c r="E82" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
+      <c r="C83" t="s">
         <v>248</v>
       </c>
-      <c r="C83" t="s">
+      <c r="D83" t="s">
         <v>249</v>
       </c>
-      <c r="D83" t="s">
+      <c r="E83" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
         <v>250</v>
       </c>
-      <c r="E83" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
+      <c r="C84" t="s">
         <v>251</v>
       </c>
-      <c r="C84" t="s">
+      <c r="D84" t="s">
         <v>252</v>
       </c>
-      <c r="D84" t="s">
+      <c r="E84" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A85" t="s">
         <v>253</v>
       </c>
-      <c r="E84" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
+      <c r="C85" t="s">
         <v>254</v>
       </c>
-      <c r="C85" t="s">
+      <c r="D85" t="s">
         <v>255</v>
       </c>
-      <c r="D85" t="s">
+      <c r="E85" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A86" t="s">
         <v>256</v>
       </c>
-      <c r="E85" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
+      <c r="C86" t="s">
         <v>257</v>
       </c>
-      <c r="C86" t="s">
+      <c r="D86" t="s">
         <v>258</v>
       </c>
-      <c r="D86" t="s">
+      <c r="E86" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A87" t="s">
         <v>259</v>
       </c>
-      <c r="E86" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
+      <c r="C87" t="s">
         <v>260</v>
       </c>
-      <c r="C87" t="s">
+      <c r="D87" t="s">
         <v>261</v>
       </c>
-      <c r="D87" t="s">
+      <c r="E87" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A88" t="s">
         <v>262</v>
       </c>
-      <c r="E87" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
+      <c r="C88" t="s">
         <v>263</v>
       </c>
-      <c r="C88" t="s">
+      <c r="D88" t="s">
         <v>264</v>
       </c>
-      <c r="D88" t="s">
+      <c r="E88" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A89" t="s">
         <v>265</v>
       </c>
-      <c r="E88" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
+      <c r="C89" t="s">
         <v>266</v>
       </c>
-      <c r="C89" t="s">
+      <c r="D89" t="s">
         <v>267</v>
       </c>
-      <c r="D89" t="s">
+      <c r="E89" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A90" t="s">
         <v>268</v>
       </c>
-      <c r="E89" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
+      <c r="C90" t="s">
         <v>269</v>
       </c>
-      <c r="C90" t="s">
+      <c r="D90" t="s">
         <v>270</v>
       </c>
-      <c r="D90" t="s">
+      <c r="E90" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A91" t="s">
         <v>271</v>
       </c>
-      <c r="E90" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
+      <c r="C91" t="s">
         <v>272</v>
       </c>
-      <c r="C91" t="s">
+      <c r="D91" t="s">
         <v>273</v>
       </c>
-      <c r="D91" t="s">
+      <c r="E91" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A92" t="s">
         <v>274</v>
       </c>
-      <c r="E91" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
+      <c r="C92" t="s">
         <v>275</v>
       </c>
-      <c r="C92" t="s">
+      <c r="D92" t="s">
         <v>276</v>
       </c>
-      <c r="D92" t="s">
+      <c r="E92" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A93" t="s">
         <v>277</v>
       </c>
-      <c r="E92" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
+      <c r="C93" t="s">
         <v>278</v>
       </c>
-      <c r="C93" t="s">
+      <c r="D93" t="s">
         <v>279</v>
-      </c>
-      <c r="D93" t="s">
-        <v>280</v>
       </c>
       <c r="E93" t="s">
         <v>8</v>

</xml_diff>